<commit_message>
fix Rx 7F for BLF
</commit_message>
<xml_diff>
--- a/scripts/PLIN-BLF.xlsx
+++ b/scripts/PLIN-BLF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\AutoAMLS\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4B401D-FCD1-47BD-92D2-17B2B2E1305C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E24F25F-CB9D-427F-AC7F-99EFB206F103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="851" firstSheet="1" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="851" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="LTT" sheetId="16" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FL_M4!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FL_M4!$A$1:$O$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FL_SX5GEV!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">FLB_SX5GEV!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">FR_M4!$A$1:$N$1</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4088" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4112" uniqueCount="449">
   <si>
     <t>SuiteName</t>
   </si>
@@ -1395,6 +1395,12 @@
   </si>
   <si>
     <t>FOR(3)</t>
+  </si>
+  <si>
+    <t>ReadS19VerionAfterFlash</t>
+  </si>
+  <si>
+    <t>22 F1 55</t>
   </si>
 </sst>
 </file>
@@ -1612,7 +1618,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1819,6 +1825,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2142,7 +2154,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2209,6 +2221,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1 2" xfId="20" xr:uid="{16881DAD-12CC-4D93-A015-B4022814418B}"/>
@@ -9751,7 +9766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5BD5C7-F362-46B8-9E4D-70C77EAB5AEF}">
   <dimension ref="A1:Y217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A136" workbookViewId="0">
       <selection activeCell="H227" sqref="H227"/>
     </sheetView>
   </sheetViews>
@@ -15377,10 +15392,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15388,19 +15403,20 @@
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -15411,40 +15427,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickTop="1">
+    <row r="2" spans="1:15" ht="15" thickTop="1">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -15454,27 +15473,28 @@
       <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>18</v>
@@ -15482,27 +15502,28 @@
       <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
+      <c r="D3" s="7"/>
       <c r="E3" s="7">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="7"/>
+      <c r="L3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="7"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>21</v>
@@ -15510,27 +15531,28 @@
       <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
+      <c r="D4" s="9"/>
       <c r="E4" s="9">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="9"/>
+      <c r="L4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="9"/>
       <c r="N4" s="9"/>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
         <v>24</v>
@@ -15538,25 +15560,26 @@
       <c r="C5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
+      <c r="D5" s="7"/>
       <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="7" t="s">
+      <c r="K5" s="7"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
         <v>27</v>
@@ -15564,25 +15587,26 @@
       <c r="C6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="9"/>
       <c r="N6" s="9"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="6"/>
       <c r="B7" s="7" t="s">
         <v>30</v>
@@ -15590,27 +15614,28 @@
       <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="7"/>
+      <c r="L7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
         <v>33</v>
@@ -15618,27 +15643,28 @@
       <c r="C8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
+      <c r="D8" s="9"/>
       <c r="E8" s="9">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="6"/>
       <c r="B9" s="7" t="s">
         <v>36</v>
@@ -15646,27 +15672,28 @@
       <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
+      <c r="D9" s="7"/>
       <c r="E9" s="7">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="7"/>
+      <c r="L9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="7"/>
       <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="7"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
         <v>39</v>
@@ -15674,27 +15701,28 @@
       <c r="C10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
+      <c r="D10" s="9"/>
       <c r="E10" s="9">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="M10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="9"/>
       <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="6" t="s">
         <v>42</v>
       </c>
@@ -15704,13 +15732,13 @@
       <c r="C11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
+      <c r="D11" s="7"/>
       <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
         <v>2</v>
       </c>
-      <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -15719,8 +15747,9 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
         <v>45</v>
@@ -15728,33 +15757,34 @@
       <c r="C12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="9">
-        <v>1</v>
-      </c>
+      <c r="D12" s="9"/>
       <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9">
         <v>2</v>
       </c>
-      <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="H12" s="9"/>
       <c r="I12" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="L12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L12" s="9"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="N12" s="9"/>
+      <c r="O12" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
         <v>51</v>
@@ -15762,33 +15792,34 @@
       <c r="C13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
+      <c r="D13" s="7"/>
       <c r="E13" s="7">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="L13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="N13" s="7"/>
+      <c r="O13" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="8"/>
       <c r="B14" s="9" t="s">
         <v>53</v>
@@ -15796,33 +15827,34 @@
       <c r="C14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="9">
-        <v>0</v>
-      </c>
+      <c r="D14" s="9"/>
       <c r="E14" s="9">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="H14" s="9"/>
       <c r="I14" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="L14" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9" t="s">
+      <c r="M14" s="9"/>
+      <c r="N14" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="6"/>
       <c r="B15" s="7" t="s">
         <v>57</v>
@@ -15830,31 +15862,32 @@
       <c r="C15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
+      <c r="D15" s="7"/>
       <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="L15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="8"/>
       <c r="B16" s="9" t="s">
         <v>59</v>
@@ -15862,31 +15895,32 @@
       <c r="C16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
+      <c r="D16" s="9"/>
       <c r="E16" s="9">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="H16" s="9"/>
       <c r="I16" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="L16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="6"/>
       <c r="B17" s="7" t="s">
         <v>62</v>
@@ -15894,33 +15928,34 @@
       <c r="C17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="7">
-        <v>0</v>
-      </c>
+      <c r="D17" s="7"/>
       <c r="E17" s="7">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="H17" s="7"/>
       <c r="I17" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="L17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="N17" s="7"/>
+      <c r="O17" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
         <v>64</v>
@@ -15928,37 +15963,38 @@
       <c r="C18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="9">
-        <v>0</v>
-      </c>
+      <c r="D18" s="9"/>
       <c r="E18" s="9">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="H18" s="9"/>
       <c r="I18" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K18" s="9" t="s">
+      <c r="L18" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="L18" s="9" t="s">
+      <c r="M18" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="N18" s="9"/>
+      <c r="O18" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="6"/>
       <c r="B19" s="7" t="s">
         <v>68</v>
@@ -15966,29 +16002,30 @@
       <c r="C19" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="7">
-        <v>0</v>
-      </c>
+      <c r="D19" s="7"/>
       <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
         <v>2</v>
       </c>
-      <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
-      <c r="K19" s="7" t="s">
+      <c r="K19" s="7"/>
+      <c r="L19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="M19" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="N19" s="7"/>
+      <c r="O19" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
         <v>71</v>
@@ -15996,535 +16033,620 @@
       <c r="C20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="9">
-        <v>0</v>
-      </c>
+      <c r="D20" s="9"/>
       <c r="E20" s="9">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9">
         <v>2</v>
       </c>
-      <c r="F20" s="9"/>
       <c r="G20" s="9"/>
-      <c r="H20" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="H20" s="9"/>
       <c r="I20" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="L20" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="6" t="s">
+      <c r="N20" s="9"/>
+      <c r="O20" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="1" customFormat="1">
+      <c r="B21" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7">
         <v>2</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="7" t="s">
+      <c r="I22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="L22" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="M22" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9" t="s">
+      <c r="N22" s="7"/>
+      <c r="O22" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C23" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="9">
-        <v>0</v>
-      </c>
-      <c r="E22" s="9">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
         <v>2</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J22" s="9" t="s">
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K23" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="L23" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9" t="s">
+      <c r="M23" s="9"/>
+      <c r="N23" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N22" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7" t="s">
+      <c r="O23" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7">
         <v>2</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J23" s="7" t="s">
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K23" s="7">
+      <c r="L24" s="7">
         <v>37</v>
       </c>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9" t="s">
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
         <v>2</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J24" s="9" t="s">
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="L25" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9" t="s">
+      <c r="M25" s="9"/>
+      <c r="N25" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N24" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7" t="s">
+      <c r="O25" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="7">
-        <v>0</v>
-      </c>
-      <c r="E25" s="7">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7">
+        <v>0</v>
+      </c>
+      <c r="F26" s="7">
         <v>2</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J25" s="7" t="s">
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="L26" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="8" t="s">
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="9">
-        <v>0</v>
-      </c>
-      <c r="E26" s="9">
+      <c r="D27" s="9"/>
+      <c r="E27" s="9">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
         <v>3</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J26" s="9" t="s">
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="K26" s="9" t="s">
+      <c r="L27" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9" t="s">
+      <c r="M27" s="9"/>
+      <c r="N27" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="N26" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7" t="s">
+      <c r="O27" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-      <c r="E27" s="7">
+      <c r="D28" s="7"/>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7">
         <v>2</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="H28" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H27" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J27" s="7" t="s">
+      <c r="I28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K27" s="7" t="s">
+      <c r="L28" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="L27" s="7" t="s">
+      <c r="M28" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9" t="s">
+      <c r="N28" s="7"/>
+      <c r="O28" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="9">
-        <v>0</v>
-      </c>
-      <c r="E28" s="9">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="9">
         <v>2</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J28" s="9" t="s">
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="L29" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9" t="s">
+      <c r="M29" s="9"/>
+      <c r="N29" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="N28" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7" t="s">
+      <c r="O29" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
+      <c r="D30" s="7"/>
+      <c r="E30" s="7">
+        <v>0</v>
+      </c>
+      <c r="F30" s="7">
         <v>2</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J29" s="7" t="s">
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K29" s="7">
+      <c r="L30" s="7">
         <v>37</v>
       </c>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9" t="s">
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="9">
-        <v>0</v>
-      </c>
-      <c r="E30" s="9">
+      <c r="D31" s="9"/>
+      <c r="E31" s="9">
+        <v>0</v>
+      </c>
+      <c r="F31" s="9">
         <v>5</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J30" s="9" t="s">
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="L31" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9" t="s">
+      <c r="M31" s="9"/>
+      <c r="N31" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N30" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="6" t="s">
+      <c r="O31" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="7">
-        <v>1</v>
-      </c>
-      <c r="E31" s="7">
+      <c r="D32" s="7"/>
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7">
         <v>2</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J31" s="7" t="s">
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="L32" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="9" t="s">
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="9">
-        <v>1</v>
-      </c>
-      <c r="E32" s="9">
+      <c r="D33" s="9"/>
+      <c r="E33" s="9">
+        <v>1</v>
+      </c>
+      <c r="F33" s="9">
         <v>2</v>
       </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J32" s="9" t="s">
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="L33" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7" t="s">
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="7">
-        <v>1</v>
-      </c>
-      <c r="E33" s="7">
+      <c r="D34" s="7"/>
+      <c r="E34" s="7">
+        <v>1</v>
+      </c>
+      <c r="F34" s="7">
         <v>2</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J33" s="7" t="s">
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K34" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K33" s="7" t="s">
+      <c r="L34" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9" t="s">
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="9">
-        <v>1</v>
-      </c>
-      <c r="E34" s="9">
+      <c r="D35" s="9"/>
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="F35" s="9">
         <v>2</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J34" s="9" t="s">
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K35" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K34" s="9">
+      <c r="L35" s="9">
         <v>14</v>
       </c>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="25"/>
+      <c r="B36" s="25" t="s">
+        <v>447</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="E36" s="25">
+        <v>0</v>
+      </c>
+      <c r="F36" s="25">
+        <v>2</v>
+      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="I36" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K36" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="L36" s="25" t="s">
+        <v>448</v>
+      </c>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16533,10 +16655,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -17180,504 +17302,533 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
+      <c r="D22" s="7">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7">
         <v>2</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="7" t="s">
+      <c r="H22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="K22" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="L22" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9" t="s">
+      <c r="M22" s="7"/>
+      <c r="N22" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C23" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="9">
-        <v>0</v>
-      </c>
-      <c r="E22" s="9">
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
         <v>2</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J22" s="9" t="s">
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K23" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9" t="s">
+      <c r="L23" s="9"/>
+      <c r="M23" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N22" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7" t="s">
+      <c r="N23" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
+      <c r="D24" s="7">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7">
         <v>2</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J23" s="7" t="s">
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K24" s="7">
         <v>37</v>
       </c>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9" t="s">
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9">
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
         <v>2</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J24" s="9" t="s">
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="K25" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9" t="s">
+      <c r="L25" s="9"/>
+      <c r="M25" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N24" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7" t="s">
+      <c r="N25" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="7">
-        <v>0</v>
-      </c>
-      <c r="E25" s="7">
+      <c r="D26" s="7">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
         <v>2</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J25" s="7" t="s">
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K26" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="8" t="s">
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="9">
-        <v>0</v>
-      </c>
-      <c r="E26" s="9">
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
         <v>3</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J26" s="9" t="s">
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="K26" s="9" t="s">
+      <c r="K27" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9" t="s">
+      <c r="L27" s="9"/>
+      <c r="M27" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="N26" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7" t="s">
+      <c r="N27" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-      <c r="E27" s="7">
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7">
         <v>2</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F28" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H27" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J27" s="7" t="s">
+      <c r="H28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K27" s="7" t="s">
+      <c r="K28" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="L27" s="7" t="s">
+      <c r="L28" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9" t="s">
+      <c r="M28" s="7"/>
+      <c r="N28" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="9">
-        <v>0</v>
-      </c>
-      <c r="E28" s="9">
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
         <v>2</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J28" s="9" t="s">
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K29" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9" t="s">
+      <c r="L29" s="9"/>
+      <c r="M29" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="N28" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7" t="s">
+      <c r="N29" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
+      <c r="E30" s="7">
         <v>2</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J29" s="7" t="s">
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K30" s="7">
         <v>37</v>
       </c>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9" t="s">
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="9">
-        <v>0</v>
-      </c>
-      <c r="E30" s="9">
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9">
         <v>5</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J30" s="9" t="s">
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K31" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9" t="s">
+      <c r="L31" s="9"/>
+      <c r="M31" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N30" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="6" t="s">
+      <c r="N31" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="7">
-        <v>1</v>
-      </c>
-      <c r="E31" s="7">
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="E32" s="7">
         <v>2</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J31" s="7" t="s">
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K32" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="9" t="s">
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="9">
-        <v>1</v>
-      </c>
-      <c r="E32" s="9">
+      <c r="D33" s="9">
+        <v>1</v>
+      </c>
+      <c r="E33" s="9">
         <v>2</v>
       </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J32" s="9" t="s">
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="K33" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7" t="s">
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="7">
-        <v>1</v>
-      </c>
-      <c r="E33" s="7">
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7">
         <v>2</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J33" s="7" t="s">
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J34" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K33" s="7" t="s">
+      <c r="K34" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9" t="s">
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="9">
-        <v>1</v>
-      </c>
-      <c r="E34" s="9">
+      <c r="D35" s="9">
+        <v>1</v>
+      </c>
+      <c r="E35" s="9">
         <v>2</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J34" s="9" t="s">
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J35" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K34" s="9">
+      <c r="K35" s="9">
         <v>14</v>
       </c>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
time cut to ~440s
</commit_message>
<xml_diff>
--- a/scripts/PLIN-BLF.xlsx
+++ b/scripts/PLIN-BLF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\AutoAMLS\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7909168A-D182-49C3-85B9-59D24C719469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E27776A-0DF1-44D2-B223-5A3E2312BAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="930" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="930" firstSheet="7" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="7" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5067" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5067" uniqueCount="487">
   <si>
     <t>SuiteName</t>
   </si>
@@ -1521,6 +1521,9 @@
   </si>
   <si>
     <t>QInputDialog</t>
+  </si>
+  <si>
+    <t>DFLZM_SX5GEV_appl_lin.s19</t>
   </si>
 </sst>
 </file>
@@ -3890,7 +3893,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4101,7 +4104,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="10" t="s">
-        <v>28</v>
+        <v>486</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>29</v>
@@ -6570,7 +6573,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B37" sqref="A37:XFD37"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6781,7 +6784,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="10" t="s">
-        <v>28</v>
+        <v>486</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>29</v>
@@ -9250,7 +9253,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9461,7 +9464,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="10" t="s">
-        <v>28</v>
+        <v>486</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>29</v>
@@ -11929,7 +11932,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O16" sqref="O15:O16"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12140,7 +12143,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="10" t="s">
-        <v>28</v>
+        <v>486</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>29</v>
@@ -13269,7 +13272,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13480,7 +13483,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="10" t="s">
-        <v>28</v>
+        <v>486</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>29</v>
@@ -14608,7 +14611,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16592,7 +16595,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O16" sqref="O15:O16"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16803,7 +16806,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="10" t="s">
-        <v>28</v>
+        <v>486</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>29</v>
@@ -19271,8 +19274,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19483,7 +19486,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="10" t="s">
-        <v>28</v>
+        <v>486</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>29</v>
@@ -26783,8 +26786,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13:P34"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
RUNIN channel and group
</commit_message>
<xml_diff>
--- a/scripts/PLIN-BLF.xlsx
+++ b/scripts/PLIN-BLF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonDev\pyside2\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonDev\AutoPlasticOmnium\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531D6DBB-C536-4079-98E3-1148663C2549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F9D471-B9C2-4314-A5F1-807E907F62C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="11" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="961" firstSheet="12" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="7" r:id="rId1"/>
@@ -42,6 +42,7 @@
     <sheet name="RMR_M4" sheetId="6" r:id="rId27"/>
     <sheet name="FRB_SX5GEV" sheetId="15" r:id="rId28"/>
     <sheet name="LTT" sheetId="16" r:id="rId29"/>
+    <sheet name="LTT1" sheetId="32" r:id="rId30"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">ALE!$A$1:$Q$33</definedName>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6069" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6209" uniqueCount="541">
   <si>
     <t>SuiteName</t>
   </si>
@@ -1657,6 +1658,45 @@
   </si>
   <si>
     <t>DFLZ_M4_appl_para.s19</t>
+  </si>
+  <si>
+    <t>ROUT Slot,Channel,On</t>
+  </si>
+  <si>
+    <t>ROUT Slot,Channel,Off</t>
+  </si>
+  <si>
+    <t>GetDAQTemp</t>
+  </si>
+  <si>
+    <t>GetDAQResistor</t>
+  </si>
+  <si>
+    <t>GetCurDev1</t>
+  </si>
+  <si>
+    <t>GetVoltDev2</t>
+  </si>
+  <si>
+    <t>Param1</t>
+  </si>
+  <si>
+    <t>ROUT 1,&lt;Channel&gt;,1</t>
+  </si>
+  <si>
+    <t>ROUT 1,&lt;Channel&gt;,0</t>
+  </si>
+  <si>
+    <t>&lt;Channel&gt;</t>
+  </si>
+  <si>
+    <t>MEASure:FRES? 100,(@10&lt;Channel&gt;)</t>
+  </si>
+  <si>
+    <t>Dev1/ai&lt;Channel&gt;</t>
+  </si>
+  <si>
+    <t>Dev2/ai&lt;Channel&gt;</t>
   </si>
 </sst>
 </file>
@@ -2811,7 +2851,655 @@
     <cellStyle name="注释 2" xfId="44" xr:uid="{F3AB96AE-817D-4279-B6C1-D2B2EF32D7CF}"/>
     <cellStyle name="警告文本 2" xfId="3" xr:uid="{645DDA24-EC4B-4017-9B81-8545B65B2980}"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="64">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFDA"/>
+          <bgColor rgb="FFE2EFDA"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2835,32 +3523,6 @@
         <patternFill patternType="solid">
           <fgColor theme="9"/>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3856,6 +4518,59 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -4566,60 +5281,85 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F7B3D7E6-E8F4-4A99-9E96-5E5CD7355C13}" name="Table3" displayName="Table3" ref="A1:Q33" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" headerRowCellStyle="常规 3" dataCellStyle="常规 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F7B3D7E6-E8F4-4A99-9E96-5E5CD7355C13}" name="Table3" displayName="Table3" ref="A1:Q33" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" headerRowCellStyle="常规 3" dataCellStyle="常规 3">
   <autoFilter ref="A1:Q33" xr:uid="{F7B3D7E6-E8F4-4A99-9E96-5E5CD7355C13}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{87D1869F-E5CC-4E60-ACD3-28ADD945AFD2}" name="SuiteName" dataDxfId="43" dataCellStyle="常规 3"/>
-    <tableColumn id="2" xr3:uid="{5B84D527-C53E-4002-8A0A-F08D9A6482FD}" name="StepName" dataDxfId="42" dataCellStyle="常规 3"/>
-    <tableColumn id="3" xr3:uid="{83EAB9B6-4C5D-44C7-AD13-97EEEFE9B22F}" name="Keyword" dataDxfId="41" dataCellStyle="常规 3"/>
-    <tableColumn id="4" xr3:uid="{89417577-A179-4EDB-BB48-8E03D52E3557}" name="Json" dataDxfId="40" dataCellStyle="常规 3"/>
-    <tableColumn id="5" xr3:uid="{1DE854ED-334F-4043-BDF8-E5AAB32D6F9F}" name="Retry" dataDxfId="39" dataCellStyle="常规 3"/>
-    <tableColumn id="6" xr3:uid="{0105D6E4-750A-46C5-9A14-11BF3C575113}" name="Timeout" dataDxfId="38" dataCellStyle="常规 3"/>
-    <tableColumn id="7" xr3:uid="{56E02C3C-624F-4D47-81FA-3EE5DC3761E9}" name="SubStr1" dataDxfId="37" dataCellStyle="常规 3"/>
-    <tableColumn id="8" xr3:uid="{0D469B1B-13E8-45EE-96CB-5060EC7A877E}" name="SubStr2" dataDxfId="36" dataCellStyle="常规 3"/>
-    <tableColumn id="9" xr3:uid="{3D4B0EC3-8C79-4453-BFB5-3333BB127BAC}" name="ID" dataDxfId="35" dataCellStyle="常规 3"/>
-    <tableColumn id="10" xr3:uid="{26E317CD-9BE1-4ACB-86D6-3FC9540DCFEB}" name="NAD" dataDxfId="34" dataCellStyle="常规 3"/>
-    <tableColumn id="11" xr3:uid="{77C4B434-6477-4B67-86E0-2565AB5F235F}" name="PCI_LEN" dataDxfId="33" dataCellStyle="常规 3"/>
-    <tableColumn id="12" xr3:uid="{F60F9C0D-C8DE-4B2B-942D-489EBC353C44}" name="CmdOrParam" dataDxfId="32" dataCellStyle="常规 3"/>
-    <tableColumn id="13" xr3:uid="{A57B0F6D-EE20-4665-8ADB-F7B477713719}" name="SetGlobalVar" dataDxfId="31" dataCellStyle="常规 3"/>
-    <tableColumn id="14" xr3:uid="{47E0619F-7A93-476C-B065-AD00DD36855A}" name="CheckStr1" dataDxfId="30" dataCellStyle="常规 3"/>
-    <tableColumn id="15" xr3:uid="{C0F86F11-1573-41FF-A474-B99BA57A8786}" name="SPEC" dataDxfId="29" dataCellStyle="常规 3"/>
-    <tableColumn id="16" xr3:uid="{0454BD28-9FF3-4377-968D-8197F5CE0D3A}" name="ByPF" dataDxfId="28" dataCellStyle="常规 3"/>
-    <tableColumn id="17" xr3:uid="{AB7C624F-B63C-451F-98DD-A9E1ECD80C4A}" name="TearDown" dataDxfId="27" dataCellStyle="常规 3"/>
+    <tableColumn id="1" xr3:uid="{87D1869F-E5CC-4E60-ACD3-28ADD945AFD2}" name="SuiteName" dataDxfId="61" dataCellStyle="常规 3"/>
+    <tableColumn id="2" xr3:uid="{5B84D527-C53E-4002-8A0A-F08D9A6482FD}" name="StepName" dataDxfId="60" dataCellStyle="常规 3"/>
+    <tableColumn id="3" xr3:uid="{83EAB9B6-4C5D-44C7-AD13-97EEEFE9B22F}" name="Keyword" dataDxfId="59" dataCellStyle="常规 3"/>
+    <tableColumn id="4" xr3:uid="{89417577-A179-4EDB-BB48-8E03D52E3557}" name="Json" dataDxfId="58" dataCellStyle="常规 3"/>
+    <tableColumn id="5" xr3:uid="{1DE854ED-334F-4043-BDF8-E5AAB32D6F9F}" name="Retry" dataDxfId="57" dataCellStyle="常规 3"/>
+    <tableColumn id="6" xr3:uid="{0105D6E4-750A-46C5-9A14-11BF3C575113}" name="Timeout" dataDxfId="56" dataCellStyle="常规 3"/>
+    <tableColumn id="7" xr3:uid="{56E02C3C-624F-4D47-81FA-3EE5DC3761E9}" name="SubStr1" dataDxfId="55" dataCellStyle="常规 3"/>
+    <tableColumn id="8" xr3:uid="{0D469B1B-13E8-45EE-96CB-5060EC7A877E}" name="SubStr2" dataDxfId="54" dataCellStyle="常规 3"/>
+    <tableColumn id="9" xr3:uid="{3D4B0EC3-8C79-4453-BFB5-3333BB127BAC}" name="ID" dataDxfId="53" dataCellStyle="常规 3"/>
+    <tableColumn id="10" xr3:uid="{26E317CD-9BE1-4ACB-86D6-3FC9540DCFEB}" name="NAD" dataDxfId="52" dataCellStyle="常规 3"/>
+    <tableColumn id="11" xr3:uid="{77C4B434-6477-4B67-86E0-2565AB5F235F}" name="PCI_LEN" dataDxfId="51" dataCellStyle="常规 3"/>
+    <tableColumn id="12" xr3:uid="{F60F9C0D-C8DE-4B2B-942D-489EBC353C44}" name="CmdOrParam" dataDxfId="50" dataCellStyle="常规 3"/>
+    <tableColumn id="13" xr3:uid="{A57B0F6D-EE20-4665-8ADB-F7B477713719}" name="SetGlobalVar" dataDxfId="49" dataCellStyle="常规 3"/>
+    <tableColumn id="14" xr3:uid="{47E0619F-7A93-476C-B065-AD00DD36855A}" name="CheckStr1" dataDxfId="48" dataCellStyle="常规 3"/>
+    <tableColumn id="15" xr3:uid="{C0F86F11-1573-41FF-A474-B99BA57A8786}" name="SPEC" dataDxfId="47" dataCellStyle="常规 3"/>
+    <tableColumn id="16" xr3:uid="{0454BD28-9FF3-4377-968D-8197F5CE0D3A}" name="ByPF" dataDxfId="46" dataCellStyle="常规 3"/>
+    <tableColumn id="17" xr3:uid="{AB7C624F-B63C-451F-98DD-A9E1ECD80C4A}" name="TearDown" dataDxfId="45" dataCellStyle="常规 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E49FA85-A79E-48ED-A160-D2BFEFA44F76}" name="Table1" displayName="Table1" ref="A1:Y217" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowCellStyle="常规 3" dataCellStyle="常规 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E49FA85-A79E-48ED-A160-D2BFEFA44F76}" name="Table1" displayName="Table1" ref="A1:Y217" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" headerRowCellStyle="常规 3" dataCellStyle="常规 3">
   <autoFilter ref="A1:Y217" xr:uid="{3E49FA85-A79E-48ED-A160-D2BFEFA44F76}"/>
   <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{4E5D4169-2B23-47E9-A636-2A629C507EAC}" name="SuiteName" dataDxfId="26" dataCellStyle="常规 3"/>
-    <tableColumn id="2" xr3:uid="{8A761701-EDCE-47BF-906F-9E38068AE090}" name="StepName" dataDxfId="25" dataCellStyle="常规 3"/>
-    <tableColumn id="3" xr3:uid="{83C1A4A7-9037-4FEE-9B43-EFC41CDCB6A5}" name="Json" dataDxfId="24" dataCellStyle="常规 3"/>
-    <tableColumn id="4" xr3:uid="{C556A570-2E18-4550-B813-7AED289DC63F}" name="Keyword" dataDxfId="23" dataCellStyle="常规 3"/>
-    <tableColumn id="5" xr3:uid="{D3A22750-A6CB-4538-A349-937F44E93036}" name="ErrorCode" dataDxfId="22" dataCellStyle="常规 3"/>
-    <tableColumn id="6" xr3:uid="{C82EF5EC-27E0-4A0B-AFD4-912756B56314}" name="Retry" dataDxfId="21" dataCellStyle="常规 3"/>
-    <tableColumn id="7" xr3:uid="{F3D9DB3D-ABC0-4D49-A31C-F35EB271275D}" name="Timeout" dataDxfId="20" dataCellStyle="常规 3"/>
-    <tableColumn id="8" xr3:uid="{9DB33ED5-A439-43E6-B49B-3B483DD102D6}" name="SubStr1" dataDxfId="19" dataCellStyle="常规 3"/>
-    <tableColumn id="9" xr3:uid="{BE830706-F564-40AC-9E83-3312E914BF41}" name="SubStr2" dataDxfId="18" dataCellStyle="常规 3"/>
-    <tableColumn id="10" xr3:uid="{CCD00695-D700-4B2E-8BD1-1BAB22C5A0C9}" name="IfElse" dataDxfId="17" dataCellStyle="常规 3"/>
-    <tableColumn id="11" xr3:uid="{E32AC69E-9472-4375-8FEE-51306ED78C3A}" name="For" dataDxfId="16" dataCellStyle="常规 3"/>
-    <tableColumn id="12" xr3:uid="{198FB01F-9F98-4F04-BBDF-A23381248D1A}" name="Model" dataDxfId="15" dataCellStyle="常规 3"/>
-    <tableColumn id="13" xr3:uid="{472AAF58-9710-4B4A-81E0-834936C4835F}" name="CmdOrParam" dataDxfId="14" dataCellStyle="常规 3"/>
-    <tableColumn id="14" xr3:uid="{107FF41C-8841-4FD5-B013-F438DC07CEA3}" name="ExpectStr" dataDxfId="13" dataCellStyle="常规 3"/>
-    <tableColumn id="15" xr3:uid="{5A5DDDAD-4DAA-45C6-B270-53DDAD9BE521}" name="CheckStr1" dataDxfId="12" dataCellStyle="常规 3"/>
-    <tableColumn id="16" xr3:uid="{544CA69B-1394-4F03-A1DD-B17B192A66EC}" name="CheckStr2" dataDxfId="11" dataCellStyle="常规 3"/>
-    <tableColumn id="17" xr3:uid="{65912A58-F1A4-4F49-8605-40A43345F077}" name="NoContain" dataDxfId="10" dataCellStyle="常规 3"/>
-    <tableColumn id="18" xr3:uid="{573F2330-DCCA-45AE-AE55-7478E3708A54}" name="SetGlobalVar" dataDxfId="9" dataCellStyle="常规 3"/>
-    <tableColumn id="19" xr3:uid="{0773A549-425E-41D7-A6ED-B909446F4536}" name="SPEC" dataDxfId="8" dataCellStyle="常规 3"/>
-    <tableColumn id="20" xr3:uid="{2A643E8D-EBCC-4E15-8BFE-E96E3FDAAE0B}" name="LSL" dataDxfId="7" dataCellStyle="常规 3"/>
-    <tableColumn id="21" xr3:uid="{3CED774E-1DBA-405B-9637-FB7DE9F309BD}" name="USL" dataDxfId="6" dataCellStyle="常规 3"/>
-    <tableColumn id="22" xr3:uid="{03F3F8CF-CBEC-416C-9895-0C104E51A070}" name="Unit" dataDxfId="5" dataCellStyle="常规 3"/>
-    <tableColumn id="23" xr3:uid="{69D6EF6E-5C93-4B3E-97B4-990B4E041002}" name="ByPF" dataDxfId="4" dataCellStyle="常规 3"/>
-    <tableColumn id="24" xr3:uid="{5E7E384D-C2B8-4839-99F0-A5710661EFEC}" name="FTC" dataDxfId="3" dataCellStyle="常规 3"/>
-    <tableColumn id="25" xr3:uid="{ADBF4FC6-951F-4EEE-8D16-E50396DAD3B4}" name="MesVar" dataDxfId="2" dataCellStyle="常规 3"/>
+    <tableColumn id="1" xr3:uid="{4E5D4169-2B23-47E9-A636-2A629C507EAC}" name="SuiteName" dataDxfId="42" dataCellStyle="常规 3"/>
+    <tableColumn id="2" xr3:uid="{8A761701-EDCE-47BF-906F-9E38068AE090}" name="StepName" dataDxfId="41" dataCellStyle="常规 3"/>
+    <tableColumn id="3" xr3:uid="{83C1A4A7-9037-4FEE-9B43-EFC41CDCB6A5}" name="Json" dataDxfId="40" dataCellStyle="常规 3"/>
+    <tableColumn id="4" xr3:uid="{C556A570-2E18-4550-B813-7AED289DC63F}" name="Keyword" dataDxfId="39" dataCellStyle="常规 3"/>
+    <tableColumn id="5" xr3:uid="{D3A22750-A6CB-4538-A349-937F44E93036}" name="ErrorCode" dataDxfId="38" dataCellStyle="常规 3"/>
+    <tableColumn id="6" xr3:uid="{C82EF5EC-27E0-4A0B-AFD4-912756B56314}" name="Retry" dataDxfId="37" dataCellStyle="常规 3"/>
+    <tableColumn id="7" xr3:uid="{F3D9DB3D-ABC0-4D49-A31C-F35EB271275D}" name="Timeout" dataDxfId="36" dataCellStyle="常规 3"/>
+    <tableColumn id="8" xr3:uid="{9DB33ED5-A439-43E6-B49B-3B483DD102D6}" name="SubStr1" dataDxfId="35" dataCellStyle="常规 3"/>
+    <tableColumn id="9" xr3:uid="{BE830706-F564-40AC-9E83-3312E914BF41}" name="SubStr2" dataDxfId="34" dataCellStyle="常规 3"/>
+    <tableColumn id="10" xr3:uid="{CCD00695-D700-4B2E-8BD1-1BAB22C5A0C9}" name="IfElse" dataDxfId="33" dataCellStyle="常规 3"/>
+    <tableColumn id="11" xr3:uid="{E32AC69E-9472-4375-8FEE-51306ED78C3A}" name="For" dataDxfId="32" dataCellStyle="常规 3"/>
+    <tableColumn id="12" xr3:uid="{198FB01F-9F98-4F04-BBDF-A23381248D1A}" name="Model" dataDxfId="31" dataCellStyle="常规 3"/>
+    <tableColumn id="13" xr3:uid="{472AAF58-9710-4B4A-81E0-834936C4835F}" name="CmdOrParam" dataDxfId="30" dataCellStyle="常规 3"/>
+    <tableColumn id="14" xr3:uid="{107FF41C-8841-4FD5-B013-F438DC07CEA3}" name="ExpectStr" dataDxfId="29" dataCellStyle="常规 3"/>
+    <tableColumn id="15" xr3:uid="{5A5DDDAD-4DAA-45C6-B270-53DDAD9BE521}" name="CheckStr1" dataDxfId="28" dataCellStyle="常规 3"/>
+    <tableColumn id="16" xr3:uid="{544CA69B-1394-4F03-A1DD-B17B192A66EC}" name="CheckStr2" dataDxfId="27" dataCellStyle="常规 3"/>
+    <tableColumn id="17" xr3:uid="{65912A58-F1A4-4F49-8605-40A43345F077}" name="NoContain" dataDxfId="26" dataCellStyle="常规 3"/>
+    <tableColumn id="18" xr3:uid="{573F2330-DCCA-45AE-AE55-7478E3708A54}" name="SetGlobalVar" dataDxfId="25" dataCellStyle="常规 3"/>
+    <tableColumn id="19" xr3:uid="{0773A549-425E-41D7-A6ED-B909446F4536}" name="SPEC" dataDxfId="24" dataCellStyle="常规 3"/>
+    <tableColumn id="20" xr3:uid="{2A643E8D-EBCC-4E15-8BFE-E96E3FDAAE0B}" name="LSL" dataDxfId="23" dataCellStyle="常规 3"/>
+    <tableColumn id="21" xr3:uid="{3CED774E-1DBA-405B-9637-FB7DE9F309BD}" name="USL" dataDxfId="22" dataCellStyle="常规 3"/>
+    <tableColumn id="22" xr3:uid="{03F3F8CF-CBEC-416C-9895-0C104E51A070}" name="Unit" dataDxfId="21" dataCellStyle="常规 3"/>
+    <tableColumn id="23" xr3:uid="{69D6EF6E-5C93-4B3E-97B4-990B4E041002}" name="ByPF" dataDxfId="20" dataCellStyle="常规 3"/>
+    <tableColumn id="24" xr3:uid="{5E7E384D-C2B8-4839-99F0-A5710661EFEC}" name="FTC" dataDxfId="19" dataCellStyle="常规 3"/>
+    <tableColumn id="25" xr3:uid="{ADBF4FC6-951F-4EEE-8D16-E50396DAD3B4}" name="MesVar" dataDxfId="18" dataCellStyle="常规 3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DD3273BC-1097-4232-BA34-0A9B4F394386}" name="Table13" displayName="Table13" ref="A1:P23" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowCellStyle="常规 3" dataCellStyle="常规 3">
+  <autoFilter ref="A1:P23" xr:uid="{3E49FA85-A79E-48ED-A160-D2BFEFA44F76}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{C53AABE7-1DC8-4C9D-BB90-5FC23616CC96}" name="SuiteName" dataDxfId="15" dataCellStyle="常规 3"/>
+    <tableColumn id="2" xr3:uid="{FF43D262-39D1-4EF5-A600-564B79840B36}" name="StepName" dataDxfId="14" dataCellStyle="常规 3"/>
+    <tableColumn id="3" xr3:uid="{4BC37492-21E1-4C3F-8E78-4E944E7B8810}" name="Json" dataDxfId="13" dataCellStyle="常规 3"/>
+    <tableColumn id="4" xr3:uid="{57B1BF8F-30F6-4693-AB47-208CEB79723D}" name="Keyword" dataDxfId="12" dataCellStyle="常规 3"/>
+    <tableColumn id="5" xr3:uid="{8C6518DA-19C5-41FE-B070-7742046ECF3B}" name="ErrorCode" dataDxfId="11" dataCellStyle="常规 3"/>
+    <tableColumn id="6" xr3:uid="{FBFE75F8-9865-4884-8CEB-BC4A44C9EFD1}" name="Retry" dataDxfId="10" dataCellStyle="常规 3"/>
+    <tableColumn id="7" xr3:uid="{B46D8C33-7B5D-48B0-AC54-DF1874ECEAAB}" name="Timeout" dataDxfId="9" dataCellStyle="常规 3"/>
+    <tableColumn id="8" xr3:uid="{9F19D014-5BA4-49AA-8461-0A8F911F2A85}" name="SubStr1" dataDxfId="8" dataCellStyle="常规 3"/>
+    <tableColumn id="9" xr3:uid="{8AC9F83D-5C93-4890-9E38-766305F376C7}" name="SubStr2" dataDxfId="7" dataCellStyle="常规 3"/>
+    <tableColumn id="11" xr3:uid="{71B5A645-36EC-45F7-8CEA-5E5903802A68}" name="For" dataDxfId="6" dataCellStyle="常规 3"/>
+    <tableColumn id="13" xr3:uid="{6CBF8460-0D5B-4EDB-8419-FC8E4F5D803F}" name="CmdOrParam" dataDxfId="5" dataCellStyle="常规 3"/>
+    <tableColumn id="14" xr3:uid="{651A7744-F728-484E-AD6E-11F426962855}" name="ExpectStr" dataDxfId="4" dataCellStyle="常规 3"/>
+    <tableColumn id="16" xr3:uid="{325C30D6-AB79-46DA-A9C0-DB50F72EECA1}" name="Param1" dataDxfId="3" dataCellStyle="常规 3"/>
+    <tableColumn id="20" xr3:uid="{3CE2081C-8C4F-493C-8153-6223A1D56529}" name="LSL" dataDxfId="2" dataCellStyle="常规 3"/>
+    <tableColumn id="21" xr3:uid="{24AF5AE9-EC6E-43A5-8D18-3D880E9B6767}" name="USL" dataDxfId="1" dataCellStyle="常规 3"/>
+    <tableColumn id="22" xr3:uid="{3CE1C27E-CE4B-4F59-981C-67AEA6D7AB23}" name="Unit" dataDxfId="0" dataCellStyle="常规 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15957,7 +16697,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -27960,8 +28700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5BD5C7-F362-46B8-9E4D-70C77EAB5AEF}">
   <dimension ref="A1:Y217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R226" sqref="R226"/>
+    <sheetView topLeftCell="A181" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M176" sqref="M176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -27973,7 +28713,8 @@
     <col min="5" max="5" width="25.5546875" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.21875" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.77734375" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" style="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.6640625" style="21" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.88671875" style="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.6640625" style="21" bestFit="1" customWidth="1"/>
@@ -37845,6 +38586,806 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DED171-53EA-4963-A620-CD38973C7186}">
+  <dimension ref="A1:P23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" style="21" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.77734375" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="M1" s="52" t="s">
+        <v>534</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="P1" s="52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="57" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>240</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="G2" s="58">
+        <v>0</v>
+      </c>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="55"/>
+      <c r="B3" s="56" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" s="56">
+        <v>1</v>
+      </c>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="57"/>
+      <c r="B4" s="58" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4" s="58">
+        <v>1</v>
+      </c>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5" s="56">
+        <v>1</v>
+      </c>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56" t="s">
+        <v>252</v>
+      </c>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="57"/>
+      <c r="B6" s="58" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="G6" s="58">
+        <v>1</v>
+      </c>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58" t="s">
+        <v>254</v>
+      </c>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="55"/>
+      <c r="B7" s="56" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" s="56">
+        <v>1</v>
+      </c>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56" t="s">
+        <v>256</v>
+      </c>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="57"/>
+      <c r="B8" s="58" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="F8" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="G8" s="58">
+        <v>1</v>
+      </c>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58" t="s">
+        <v>258</v>
+      </c>
+      <c r="L8" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="58"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="55"/>
+      <c r="B9" s="56" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="G9" s="56">
+        <v>1</v>
+      </c>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56" t="s">
+        <v>260</v>
+      </c>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="57"/>
+      <c r="B10" s="58" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="58">
+        <v>1</v>
+      </c>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58" t="s">
+        <v>262</v>
+      </c>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+    </row>
+    <row r="11" spans="1:16" ht="15" thickBot="1">
+      <c r="A11" s="55"/>
+      <c r="B11" s="56" t="s">
+        <v>263</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" s="56">
+        <v>1</v>
+      </c>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56" t="s">
+        <v>264</v>
+      </c>
+      <c r="L11" s="56" t="s">
+        <v>265</v>
+      </c>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" thickTop="1">
+      <c r="A12" s="53" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54">
+        <v>3</v>
+      </c>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="L12" s="54">
+        <v>9600</v>
+      </c>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="57"/>
+      <c r="B13" s="58" t="s">
+        <v>528</v>
+      </c>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="58">
+        <v>1</v>
+      </c>
+      <c r="G13" s="58">
+        <v>1</v>
+      </c>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58" t="s">
+        <v>535</v>
+      </c>
+      <c r="L13" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="55" t="s">
+        <v>416</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56">
+        <v>3</v>
+      </c>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="L14" s="56">
+        <v>9600</v>
+      </c>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="55"/>
+      <c r="B15" s="56" t="s">
+        <v>529</v>
+      </c>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="56">
+        <v>1</v>
+      </c>
+      <c r="G15" s="56">
+        <v>1</v>
+      </c>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56" t="s">
+        <v>536</v>
+      </c>
+      <c r="L15" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="57" t="s">
+        <v>439</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>440</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58" t="s">
+        <v>440</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="F16" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="G16" s="58">
+        <v>1</v>
+      </c>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58" t="s">
+        <v>441</v>
+      </c>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="55" t="s">
+        <v>433</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="G17" s="56">
+        <v>1</v>
+      </c>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56" t="s">
+        <v>267</v>
+      </c>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="55"/>
+      <c r="B18" s="56" t="s">
+        <v>530</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F18" s="56">
+        <v>0</v>
+      </c>
+      <c r="G18" s="56">
+        <v>3</v>
+      </c>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="56" t="s">
+        <v>269</v>
+      </c>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56" t="s">
+        <v>537</v>
+      </c>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="57" t="s">
+        <v>434</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>331</v>
+      </c>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="E19" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="F19" s="58">
+        <v>0</v>
+      </c>
+      <c r="G19" s="58">
+        <v>1</v>
+      </c>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58" t="s">
+        <v>332</v>
+      </c>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="57"/>
+      <c r="B20" s="58" t="s">
+        <v>531</v>
+      </c>
+      <c r="C20" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="F20" s="58">
+        <v>0</v>
+      </c>
+      <c r="G20" s="58">
+        <v>3</v>
+      </c>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58" t="s">
+        <v>333</v>
+      </c>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58" t="s">
+        <v>538</v>
+      </c>
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="58"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="55" t="s">
+        <v>435</v>
+      </c>
+      <c r="B21" s="56" t="s">
+        <v>532</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>336</v>
+      </c>
+      <c r="E21" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F21" s="56">
+        <v>0</v>
+      </c>
+      <c r="G21" s="56">
+        <v>10</v>
+      </c>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56" t="s">
+        <v>539</v>
+      </c>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56" t="s">
+        <v>338</v>
+      </c>
+      <c r="O21" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="P21" s="56" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="55" t="s">
+        <v>436</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>533</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>376</v>
+      </c>
+      <c r="E22" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F22" s="56">
+        <v>0</v>
+      </c>
+      <c r="G22" s="56">
+        <v>10</v>
+      </c>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56" t="s">
+        <v>540</v>
+      </c>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56">
+        <v>-20</v>
+      </c>
+      <c r="O22" s="56">
+        <v>30</v>
+      </c>
+      <c r="P22" s="56" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="55" t="s">
+        <v>438</v>
+      </c>
+      <c r="B23" s="56" t="s">
+        <v>437</v>
+      </c>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56" t="s">
+        <v>413</v>
+      </c>
+      <c r="E23" s="56" t="s">
+        <v>414</v>
+      </c>
+      <c r="F23" s="56">
+        <v>0</v>
+      </c>
+      <c r="G23" s="56">
+        <v>10</v>
+      </c>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>

</xml_diff>

<commit_message>
add flow control ico
</commit_message>
<xml_diff>
--- a/scripts/PLIN-BLF.xlsx
+++ b/scripts/PLIN-BLF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonDev\AutoPlasticOmnium\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E2E250-6148-407A-A2E0-165D5933B975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047029BB-AE76-4354-B277-7E4F3EBFDBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="351">
   <si>
     <t>SuiteName</t>
   </si>
@@ -1066,13 +1066,31 @@
   </si>
   <si>
     <t>ShowVersionAfterFlash</t>
+  </si>
+  <si>
+    <t>IfElse</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>elif</t>
+  </si>
+  <si>
+    <t>&amp;if</t>
+  </si>
+  <si>
+    <t>||if</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1273,6 +1291,12 @@
       <color theme="1"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1751,7 +1775,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="24" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1785,6 +1809,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
@@ -1963,9 +1988,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="M4" displayName="M4_" ref="A1:P42">
-  <autoFilter ref="A1:P42" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="M4" displayName="M4_" ref="A1:Q42">
+  <autoFilter ref="A1:Q42" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="SuiteName"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="StepName"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Keyword"/>
@@ -1973,6 +1998,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Timeout"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="SubStr1"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="SubStr2"/>
+    <tableColumn id="18" xr3:uid="{81FD3D3F-B221-4A71-A13F-61537B5EA5F9}" name="IfElse"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Model"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="ID"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="NAD"/>
@@ -5727,10 +5753,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -5741,7 +5767,7 @@
     <col min="4" max="4" width="8.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" style="10" customWidth="1"/>
     <col min="9" max="9" width="5.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.77734375" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.21875" style="10" bestFit="1" customWidth="1"/>
@@ -5754,7 +5780,7 @@
     <col min="31" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5776,35 +5802,38 @@
       <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="I1" t="s">
         <v>143</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>106</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>107</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>108</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>144</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>109</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="2" spans="1:17" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>145</v>
       </c>
@@ -5820,17 +5849,17 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>148</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>116</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="3" spans="1:17" ht="15" customHeight="1">
       <c r="B3" t="s">
         <v>146</v>
       </c>
@@ -5843,17 +5872,17 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>149</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>125</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="4" spans="1:17" ht="15" customHeight="1">
       <c r="B4" t="s">
         <v>146</v>
       </c>
@@ -5866,17 +5895,17 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>150</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>127</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="5" spans="1:17" ht="15" customHeight="1">
       <c r="B5" t="s">
         <v>146</v>
       </c>
@@ -5889,17 +5918,20 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="I5" t="s">
         <v>151</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>129</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="6" spans="1:17" ht="15" customHeight="1">
       <c r="B6" t="s">
         <v>146</v>
       </c>
@@ -5912,17 +5944,20 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="I6" t="s">
         <v>152</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>131</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1">
+    <row r="7" spans="1:17" ht="15" customHeight="1">
       <c r="B7" t="s">
         <v>146</v>
       </c>
@@ -5935,17 +5970,20 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="I7" t="s">
         <v>153</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>133</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="B8" t="s">
         <v>154</v>
       </c>
@@ -5958,14 +5996,17 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="L8" t="s">
+      <c r="H8" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="M8" t="s">
         <v>155</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="B9" t="s">
         <v>157</v>
       </c>
@@ -5978,14 +6019,17 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="L9" t="s">
+      <c r="H9" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M9" t="s">
         <v>159</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="B10" t="s">
         <v>161</v>
       </c>
@@ -5998,14 +6042,17 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="L10" t="s">
+      <c r="H10" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M10" t="s">
         <v>159</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="B11" t="s">
         <v>164</v>
       </c>
@@ -6018,14 +6065,17 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="L11" t="s">
+      <c r="H11" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M11" t="s">
         <v>166</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="B12" t="s">
         <v>168</v>
       </c>
@@ -6038,14 +6088,14 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>169</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="B13" t="s">
         <v>171</v>
       </c>
@@ -6058,14 +6108,14 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>172</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="B14" t="s">
         <v>174</v>
       </c>
@@ -6078,14 +6128,14 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>172</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="B15" t="s">
         <v>176</v>
       </c>
@@ -6098,14 +6148,14 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>177</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
       <c r="B16" t="s">
         <v>179</v>
       </c>
@@ -6118,14 +6168,14 @@
       <c r="E16">
         <v>2</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>159</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>180</v>
       </c>
@@ -6142,7 +6192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="B18" t="s">
         <v>113</v>
       </c>
@@ -6155,20 +6205,20 @@
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>115</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>181</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>117</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="B19" t="s">
         <v>343</v>
       </c>
@@ -6187,26 +6237,26 @@
       <c r="G19" t="s">
         <v>121</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>115</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>181</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>122</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>123</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>124</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="B20" t="s">
         <v>182</v>
       </c>
@@ -6219,20 +6269,20 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>115</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>181</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>117</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="B21" t="s">
         <v>184</v>
       </c>
@@ -6245,23 +6295,23 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>115</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>181</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>185</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>186</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="B22" t="s">
         <v>340</v>
       </c>
@@ -6274,20 +6324,20 @@
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>115</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>181</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>117</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="B23" t="s">
         <v>341</v>
       </c>
@@ -6300,20 +6350,20 @@
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>115</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>181</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>122</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="B24" t="s">
         <v>342</v>
       </c>
@@ -6326,20 +6376,20 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>115</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>181</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>117</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="B25" t="s">
         <v>191</v>
       </c>
@@ -6355,23 +6405,23 @@
       <c r="F25" t="s">
         <v>192</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>115</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>181</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>117</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>193</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17">
       <c r="B26" t="s">
         <v>195</v>
       </c>
@@ -6384,14 +6434,14 @@
       <c r="E26">
         <v>2</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>196</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17">
       <c r="B27" t="s">
         <v>198</v>
       </c>
@@ -6404,20 +6454,20 @@
       <c r="E27">
         <v>2</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>115</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>181</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>199</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>201</v>
       </c>
@@ -6439,23 +6489,23 @@
       <c r="G28" t="s">
         <v>121</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>115</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>181</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>205</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>206</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17">
       <c r="B29" t="s">
         <v>208</v>
       </c>
@@ -6468,23 +6518,23 @@
       <c r="E29">
         <v>2</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>115</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>181</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>209</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>172</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17">
       <c r="B30" t="s">
         <v>211</v>
       </c>
@@ -6497,20 +6547,20 @@
       <c r="E30">
         <v>2</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>115</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>181</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>212</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:17">
       <c r="B31" t="s">
         <v>214</v>
       </c>
@@ -6523,23 +6573,23 @@
       <c r="E31">
         <v>2</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>115</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>181</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>215</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>216</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:17">
       <c r="B32" t="s">
         <v>218</v>
       </c>
@@ -6552,20 +6602,20 @@
       <c r="E32">
         <v>2</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>115</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>181</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>219</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>221</v>
       </c>
@@ -6581,23 +6631,23 @@
       <c r="E33">
         <v>3</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>115</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>181</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>223</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>224</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17">
       <c r="B34" t="s">
         <v>202</v>
       </c>
@@ -6616,23 +6666,23 @@
       <c r="G34" t="s">
         <v>121</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>115</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>181</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>205</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>226</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:17">
       <c r="B35" t="s">
         <v>208</v>
       </c>
@@ -6645,23 +6695,23 @@
       <c r="E35">
         <v>2</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>115</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>181</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>209</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>159</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:17">
       <c r="B36" t="s">
         <v>211</v>
       </c>
@@ -6674,20 +6724,20 @@
       <c r="E36">
         <v>2</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>115</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>181</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>212</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:17">
       <c r="B37" t="s">
         <v>214</v>
       </c>
@@ -6700,23 +6750,23 @@
       <c r="E37">
         <v>5</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>115</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>181</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>215</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>228</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>229</v>
       </c>
@@ -6732,20 +6782,20 @@
       <c r="E38">
         <v>2</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>115</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>181</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>185</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:17">
       <c r="B39" t="s">
         <v>113</v>
       </c>
@@ -6758,20 +6808,20 @@
       <c r="E39">
         <v>2</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>115</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>181</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>117</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:17">
       <c r="B40" t="s">
         <v>232</v>
       </c>
@@ -6784,20 +6834,20 @@
       <c r="E40">
         <v>2</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>115</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>181</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>117</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:17">
       <c r="B41" t="s">
         <v>234</v>
       </c>
@@ -6810,20 +6860,20 @@
       <c r="E41">
         <v>2</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>115</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>181</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>185</v>
       </c>
-      <c r="L41" t="s">
+      <c r="M41" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:17">
       <c r="B42" t="s">
         <v>344</v>
       </c>
@@ -6842,26 +6892,28 @@
       <c r="G42" t="s">
         <v>121</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>115</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>181</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>122</v>
       </c>
-      <c r="L42" t="s">
+      <c r="M42" t="s">
         <v>123</v>
       </c>
-      <c r="P42" t="s">
+      <c r="Q42" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7973,7 +8025,7 @@
   </sheetPr>
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>

</xml_diff>